<commit_message>
Update: Excel Reporting FINISHED
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/tableList.xlsx
+++ b/src/test/resources/Excel/tableList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kar.par\Documents\GitHub\ThirdPartyAutomation\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A80D56-0B86-4647-9DCF-30E17AD81D94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C057E6E9-B5AA-4A42-BF48-3636B4B940C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5370" yWindow="1830" windowWidth="22245" windowHeight="12615" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5775" yWindow="810" windowWidth="22245" windowHeight="12615" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="1" r:id="rId1"/>
@@ -1575,9 +1575,6 @@
     <t>TableC03</t>
   </si>
   <si>
-    <t>Table C07</t>
-  </si>
-  <si>
     <t>Table31</t>
   </si>
   <si>
@@ -1590,12 +1587,6 @@
     <t>Table72</t>
   </si>
   <si>
-    <t>Table C06</t>
-  </si>
-  <si>
-    <t>Table C05</t>
-  </si>
-  <si>
     <t>Table10</t>
   </si>
   <si>
@@ -1605,14 +1596,23 @@
     <t>TableC01</t>
   </si>
   <si>
-    <t>Table C04</t>
+    <t>TableC06</t>
+  </si>
+  <si>
+    <t>TableC05</t>
+  </si>
+  <si>
+    <t>TableC04</t>
+  </si>
+  <si>
+    <t>TableC07</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1645,6 +1645,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1672,7 +1679,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1691,6 +1698,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7488,7 +7501,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7741,8 +7754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F8A6884-001C-4D75-8C17-13F9358C07DC}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7962,27 +7975,28 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>484</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="8" t="s">
         <v>415</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="8" t="s">
         <v>498</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="8" t="s">
         <v>406</v>
       </c>
     </row>
@@ -7991,13 +8005,13 @@
         <v>499</v>
       </c>
       <c r="B2" t="s">
+        <v>510</v>
+      </c>
+      <c r="C2" t="s">
         <v>511</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>512</v>
-      </c>
-      <c r="D2" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -8005,10 +8019,10 @@
         <v>500</v>
       </c>
       <c r="B3" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="D3" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -8048,12 +8062,12 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -8068,26 +8082,27 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>510</v>
+        <v>520</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update: Sexy Gaming Tables Added
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/tableList.xlsx
+++ b/src/test/resources/Excel/tableList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kar.par\Documents\GitHub\ThirdPartyAutomation\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12DD842-4C54-4342-98FA-15C6092814A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE29A3E8-0214-4B5C-9713-81C47890908C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="1005" windowWidth="25050" windowHeight="13320" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31065" yWindow="1245" windowWidth="25050" windowHeight="13320" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1691" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1694" uniqueCount="528">
   <si>
     <t>3RD PARTY</t>
   </si>
@@ -1618,6 +1618,15 @@
   </si>
   <si>
     <t>Roulette Azure</t>
+  </si>
+  <si>
+    <t>TableC08</t>
+  </si>
+  <si>
+    <t>TableC09</t>
+  </si>
+  <si>
+    <t>TableC10</t>
   </si>
 </sst>
 </file>
@@ -7526,7 +7535,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B397D14-7939-4B63-AABD-1966ADACE430}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -8019,10 +8028,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77F0C1E1-6152-495F-801F-3660D0C2A57D}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8147,6 +8156,21 @@
         <v>515</v>
       </c>
     </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>527</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>